<commit_message>
Finalize v1.0 invoice automation release
</commit_message>
<xml_diff>
--- a/sample-data/Input/VendorMaster.xlsx
+++ b/sample-data/Input/VendorMaster.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/33650d8d57f62057/Desktop/BP_InvoiceBot/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/33650d8d57f62057/Desktop/invoice-automation-blueprism/sample-data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C19E30AA-073A-42C2-9156-B7E685E46A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{C19E30AA-073A-42C2-9156-B7E685E46A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FEBCECF-3DB8-4CB4-99C1-FA691992E133}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A4F515A8-1459-4ABF-AE9B-D1130C058BBC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
   <si>
     <t>VendorName</t>
   </si>
@@ -183,6 +183,42 @@
   </si>
   <si>
     <t>V022</t>
+  </si>
+  <si>
+    <t>Adventure Works Training</t>
+  </si>
+  <si>
+    <t>Litware Utilities</t>
+  </si>
+  <si>
+    <t>Northwind Office Supplies</t>
+  </si>
+  <si>
+    <t>Tailspin Logistics</t>
+  </si>
+  <si>
+    <t>V023</t>
+  </si>
+  <si>
+    <t>V024</t>
+  </si>
+  <si>
+    <t>V025</t>
+  </si>
+  <si>
+    <t>V026</t>
+  </si>
+  <si>
+    <t>V027</t>
+  </si>
+  <si>
+    <t>V028</t>
+  </si>
+  <si>
+    <t>Contoso IT Services Inc.</t>
+  </si>
+  <si>
+    <t>Fabrikam Facilities Co.</t>
   </si>
 </sst>
 </file>
@@ -257,6 +293,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,15 +616,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259154F1-B3E9-4E85-B789-0E0F09F15C85}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -842,6 +880,72 @@
         <v>6</v>
       </c>
     </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>